<commit_message>
Commit 2 16th May
</commit_message>
<xml_diff>
--- a/03_plots_and_tables/accuracy_all.xlsx
+++ b/03_plots_and_tables/accuracy_all.xlsx
@@ -381,7 +381,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>0.876854599406528</v>
+        <v>0.878338278931751</v>
       </c>
       <c r="C2">
         <v>0.888724035608309</v>
@@ -397,7 +397,7 @@
         <v>0.847181008902077</v>
       </c>
       <c r="C3">
-        <v>0.862017804154303</v>
+        <v>0.859050445103858</v>
       </c>
     </row>
     <row r="4">
@@ -407,7 +407,7 @@
         </is>
       </c>
       <c r="B4">
-        <v>0.841246290801187</v>
+        <v>0.836795252225519</v>
       </c>
       <c r="C4">
         <v>0.851632047477745</v>
@@ -420,49 +420,49 @@
         </is>
       </c>
       <c r="B5">
-        <v>0.836795252225519</v>
+        <v>0.835311572700297</v>
       </c>
       <c r="C5">
-        <v>0.863501483679525</v>
+        <v>0.86646884272997</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>margalef + gini_index</t>
+          <t>fisher_alpha + gini_index</t>
         </is>
       </c>
       <c r="B6">
-        <v>0.832344213649852</v>
+        <v>0.829376854599407</v>
       </c>
       <c r="C6">
-        <v>0.850148367952522</v>
+        <v>0.853115727002967</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>fisher_alpha + gini_index</t>
+          <t>margalef + gini_index</t>
         </is>
       </c>
       <c r="B7">
-        <v>0.830860534124629</v>
+        <v>0.8234421364985161</v>
       </c>
       <c r="C7">
-        <v>0.85459940652819</v>
+        <v>0.850148367952522</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>menhinick + strong</t>
+          <t>chao1 + pielou_evenness</t>
         </is>
       </c>
       <c r="B8">
-        <v>0.731454005934718</v>
+        <v>0.7195845697329381</v>
       </c>
       <c r="C8">
-        <v>0.747774480712166</v>
+        <v>0.743323442136498</v>
       </c>
     </row>
     <row r="9">
@@ -472,85 +472,85 @@
         </is>
       </c>
       <c r="B9">
-        <v>0.724035608308605</v>
+        <v>0.7195845697329381</v>
       </c>
       <c r="C9">
-        <v>0.755192878338279</v>
+        <v>0.741839762611276</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>menhinick + pielou_evenness</t>
+          <t>menhinick + strong</t>
         </is>
       </c>
       <c r="B10">
-        <v>0.724035608308605</v>
+        <v>0.716617210682493</v>
       </c>
       <c r="C10">
-        <v>0.753709198813056</v>
+        <v>0.737388724035608</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>chao1 + pielou_evenness</t>
+          <t>menhinick + pielou_evenness</t>
         </is>
       </c>
       <c r="B11">
-        <v>0.722551928783383</v>
+        <v>0.713649851632048</v>
       </c>
       <c r="C11">
-        <v>0.758160237388724</v>
+        <v>0.732937685459941</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>margalef + simpson</t>
+          <t>menhinick + shannon_entropy</t>
         </is>
       </c>
       <c r="B12">
+        <v>0.70919881305638</v>
+      </c>
+      <c r="C12">
         <v>0.722551928783383</v>
-      </c>
-      <c r="C12">
-        <v>0.737388724035608</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>faith_pd + pielou_evenness</t>
+          <t>fisher_alpha + pielou_evenness</t>
         </is>
       </c>
       <c r="B13">
-        <v>0.722551928783383</v>
+        <v>0.70919881305638</v>
       </c>
       <c r="C13">
-        <v>0.724035608308605</v>
+        <v>0.737388724035608</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>fisher_alpha + pielou_evenness</t>
+          <t>fisher_alpha + shannon_entropy</t>
         </is>
       </c>
       <c r="B14">
-        <v>0.7195845697329381</v>
+        <v>0.707715133531157</v>
       </c>
       <c r="C14">
-        <v>0.746290801186944</v>
+        <v>0.729970326409496</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>fisher_alpha + shannon_entropy</t>
+          <t>margalef + shannon_entropy</t>
         </is>
       </c>
       <c r="B15">
-        <v>0.7181008902077149</v>
+        <v>0.704747774480712</v>
       </c>
       <c r="C15">
         <v>0.737388724035608</v>
@@ -559,50 +559,50 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>menhinick + shannon_entropy</t>
+          <t>margalef + pielou_evenness</t>
         </is>
       </c>
       <c r="B16">
-        <v>0.716617210682493</v>
+        <v>0.6988130563798221</v>
       </c>
       <c r="C16">
-        <v>0.744807121661721</v>
+        <v>0.734421364985163</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>margalef + pielou_evenness</t>
+          <t>margalef + simpson</t>
         </is>
       </c>
       <c r="B17">
-        <v>0.70919881305638</v>
+        <v>0.6988130563798221</v>
       </c>
       <c r="C17">
-        <v>0.744807121661721</v>
+        <v>0.732937685459941</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>margalef + shannon_entropy</t>
+          <t>faith_pd + pielou_evenness</t>
         </is>
       </c>
       <c r="B18">
-        <v>0.707715133531157</v>
+        <v>0.694362017804154</v>
       </c>
       <c r="C18">
-        <v>0.732937685459941</v>
+        <v>0.704747774480712</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>fisher_alpha + strong</t>
+          <t>chao1 + shannon_entropy</t>
         </is>
       </c>
       <c r="B19">
-        <v>0.704747774480712</v>
+        <v>0.692878338278932</v>
       </c>
       <c r="C19">
         <v>0.72700296735905</v>
@@ -611,92 +611,92 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>faith_pd + simpson</t>
+          <t>fisher_alpha + simpson</t>
         </is>
       </c>
       <c r="B20">
-        <v>0.70326409495549</v>
+        <v>0.689910979228487</v>
       </c>
       <c r="C20">
-        <v>0.7181008902077149</v>
+        <v>0.706231454005935</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>chao1 + shannon_entropy</t>
+          <t>menhinick + simpson</t>
         </is>
       </c>
       <c r="B21">
-        <v>0.700296735905044</v>
+        <v>0.682492581602374</v>
       </c>
       <c r="C21">
-        <v>0.7403560830860531</v>
+        <v>0.706231454005935</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>menhinick + simpson</t>
+          <t>chao1 + strong</t>
         </is>
       </c>
       <c r="B22">
-        <v>0.700296735905044</v>
+        <v>0.6780415430267061</v>
       </c>
       <c r="C22">
-        <v>0.72106824925816</v>
+        <v>0.724035608308605</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>fisher_alpha + simpson</t>
+          <t>margalef + strong</t>
         </is>
       </c>
       <c r="B23">
-        <v>0.6988130563798221</v>
+        <v>0.6765578635014839</v>
       </c>
       <c r="C23">
-        <v>0.735905044510386</v>
+        <v>0.712166172106825</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>margalef + strong</t>
+          <t>faith_pd + shannon_entropy</t>
         </is>
       </c>
       <c r="B24">
-        <v>0.695845697329377</v>
+        <v>0.6765578635014839</v>
       </c>
       <c r="C24">
-        <v>0.72700296735905</v>
+        <v>0.683976261127596</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>chao1 + strong</t>
+          <t>faith_pd + simpson</t>
         </is>
       </c>
       <c r="B25">
-        <v>0.689910979228487</v>
+        <v>0.675074183976261</v>
       </c>
       <c r="C25">
-        <v>0.732937685459941</v>
+        <v>0.695845697329377</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>faith_pd + shannon_entropy</t>
+          <t>fisher_alpha + strong</t>
         </is>
       </c>
       <c r="B26">
-        <v>0.689910979228487</v>
+        <v>0.670623145400593</v>
       </c>
       <c r="C26">
-        <v>0.6973293768545989</v>
+        <v>0.713649851632048</v>
       </c>
     </row>
     <row r="27">
@@ -706,10 +706,10 @@
         </is>
       </c>
       <c r="B27">
-        <v>0.667655786350148</v>
+        <v>0.642433234421365</v>
       </c>
       <c r="C27">
-        <v>0.675074183976261</v>
+        <v>0.663204747774481</v>
       </c>
     </row>
   </sheetData>

</xml_diff>